<commit_message>
Adding IBM Load Sharing Facility Conversion Rules using the Control-M Self Conversion
</commit_message>
<xml_diff>
--- a/Load Sharing Facility/MappingLogic.xlsx
+++ b/Load Sharing Facility/MappingLogic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DimaData\SelfC\Load Sharing Facility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshoofy\git\self-conversion-api-community-solutions\Load Sharing Facility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A564E246-8B63-434C-BBFC-7D53A285BFD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D245C2-F8DB-4EAF-A207-22FA0B0BDFC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4EB21CC8-22F2-410E-8299-C48C4A5CC6ED}"/>
+    <workbookView xWindow="6165" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{4EB21CC8-22F2-410E-8299-C48C4A5CC6ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>Control-M Data</t>
   </si>
   <si>
-    <t>Smart Folder</t>
-  </si>
-  <si>
     <t>Smart Folder Name</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Name of the Entity that raise Out Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smart Folder </t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -525,82 +525,82 @@
     </row>
     <row r="2" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>